<commit_message>
changed Data in excel for UserSkillMap & skills
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/InputData_UserSkillsMap.xlsx
+++ b/src/test/resources/TestData/InputData_UserSkillsMap.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A13E1E72-912A-4AFF-867A-95463668BB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{5CB58FF9-20EF-47A0-B6E2-8779D6F17450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8388" yWindow="480" windowWidth="14640" windowHeight="8964" activeTab="2" xr2:uid="{0AC15290-BAA0-473B-840B-AEEDC9E05017}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="14712" windowHeight="13224" firstSheet="2" activeTab="2" xr2:uid="{0AC15290-BAA0-473B-840B-AEEDC9E05017}"/>
   </bookViews>
   <sheets>
     <sheet name="InputData_UserSkillsMap_userGET" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Scenario</t>
   </si>
@@ -31,9 +31,6 @@
     <t>StatusCode</t>
   </si>
   <si>
-    <t>Status_Message</t>
-  </si>
-  <si>
     <t>GET method for valid User ID</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Skill not found</t>
   </si>
   <si>
-    <t>skill_id</t>
-  </si>
-  <si>
     <t>GET method for non-existing skill ID</t>
   </si>
   <si>
@@ -119,6 +113,9 @@
   </si>
   <si>
     <t>To Check Authorization with valid username and password</t>
+  </si>
+  <si>
+    <t>Skill_Id</t>
   </si>
 </sst>
 </file>
@@ -520,7 +517,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -537,21 +534,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>200</v>
@@ -559,44 +556,44 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C3" s="1">
         <v>404</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>404</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>404</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -616,75 +613,75 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.4" thickBot="1">
       <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="115.8" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>401</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="115.8" thickBot="1">
       <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D3">
         <v>401</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="115.8" thickBot="1">
       <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D4">
         <v>401</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="101.4" thickBot="1">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>200</v>
@@ -705,7 +702,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -721,18 +718,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -744,7 +741,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>200</v>
@@ -753,35 +750,35 @@
         <v>404</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>404</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2">
         <v>404</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>